<commit_message>
Gaby time sheet and attendance updates
</commit_message>
<xml_diff>
--- a/Admin/Gaby/spring/TimeSheet_Week1.xlsx
+++ b/Admin/Gaby/spring/TimeSheet_Week1.xlsx
@@ -103,7 +103,7 @@
     <numFmt numFmtId="165" formatCode="d\-mmm"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,13 +133,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -229,11 +222,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -262,10 +255,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,7 +279,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -375,10 +364,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -446,257 +435,261 @@
       <c r="B5" s="6" t="n">
         <v>44571</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>44572</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>44573</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>44574</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>44575</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>44576</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="6" t="n">
         <v>44577</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="9"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="13" t="n">
+      <c r="B6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="12" t="n">
         <f aca="false">SUM(B6:H6)</f>
         <v>1</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13" t="n">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="12" t="n">
         <f aca="false">SUM(B7:H7)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="13" t="n">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="12" t="n">
         <f aca="false">SUM(B8:H8)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="9"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13" t="n">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="12" t="n">
         <f aca="false">SUM(B9:H9)</f>
         <v>1</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="13" t="n">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="12" t="n">
         <f aca="false">SUM(B10:H10)</f>
         <v>1</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="13" t="n">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="12" t="n">
         <f aca="false">SUM(B11:H11)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="13" t="n">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="12" t="n">
         <f aca="false">SUM(B12:H12)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13" t="n">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="12" t="n">
         <f aca="false">SUM(B13:H13)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13" t="n">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="n">
         <f aca="false">SUM(B14:H14)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="13" t="n">
+      <c r="B15" s="12" t="n">
         <f aca="false">SUM(B6:B14)</f>
         <v>1</v>
       </c>
-      <c r="C15" s="13" t="n">
+      <c r="C15" s="12" t="n">
         <f aca="false">SUM(C6:C14)</f>
         <v>2</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="12" t="n">
         <f aca="false">SUM(D6:D14)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="13" t="n">
+      <c r="E15" s="12" t="n">
         <f aca="false">SUM(E6:E14)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12" t="n">
         <f aca="false">SUM(F6:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="13" t="n">
+      <c r="G15" s="12" t="n">
         <f aca="false">SUM(G6:G14)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="13" t="n">
+      <c r="H15" s="12" t="n">
         <f aca="false">SUM(H6:H14)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12" t="n">
         <f aca="false">SUM(I6:I14)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>